<commit_message>
Optimizations for Icao9303Algorithm and Icao9303SizeTD3Algorithm. Benchmarks for Icao9303SizeTD3Algorithm
</commit_message>
<xml_diff>
--- a/Documentation/ICAO9303ExamplesWorkbook.xlsx
+++ b/Documentation/ICAO9303ExamplesWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53A781-4E20-4F71-B21D-A32C881781A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC2A28-AF27-45E9-8769-89F8D5FA0981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{733EF23D-49B3-4624-B260-D0D00364A32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
   <si>
     <t>Char</t>
   </si>
@@ -111,6 +111,39 @@
   </si>
   <si>
     <t>&lt;</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -504,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7BF346-6A22-4B48-81BB-0FB387D62345}">
-  <dimension ref="A2:K128"/>
+  <dimension ref="A2:K171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,7 +3048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>12</v>
       </c>
@@ -3048,7 +3081,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>13</v>
       </c>
@@ -3081,7 +3114,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>14</v>
       </c>
@@ -3114,7 +3147,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -3139,7 +3172,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -3148,134 +3181,2629 @@
       </c>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="3"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="3"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C91" s="3"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="3"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="3"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="3"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C95" s="3"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="3"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="3"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="3"/>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="3"/>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="3"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="3"/>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="3"/>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="3"/>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="3"/>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="3"/>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="3"/>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="3"/>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="3"/>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="3"/>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="3"/>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C111" s="3"/>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C112" s="3"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="3"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="3"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="3"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="3"/>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="3"/>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="3"/>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C119" s="3"/>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C121" s="3"/>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="3"/>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C123" s="3"/>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="3"/>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="3"/>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C126" s="3"/>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="3"/>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" s="2"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89">
+        <v>26</v>
+      </c>
+      <c r="E89">
+        <v>7</v>
+      </c>
+      <c r="F89">
+        <f>D89*E89</f>
+        <v>182</v>
+      </c>
+      <c r="G89">
+        <f>F89</f>
+        <v>182</v>
+      </c>
+      <c r="H89">
+        <v>7</v>
+      </c>
+      <c r="I89">
+        <f>D89*H89</f>
+        <v>182</v>
+      </c>
+      <c r="J89">
+        <f>I89</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" s="3">
+        <v>1</v>
+      </c>
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>3</v>
+      </c>
+      <c r="F90">
+        <f t="shared" ref="F90:F97" si="29">D90*E90</f>
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <f>G89+F90</f>
+        <v>185</v>
+      </c>
+      <c r="H90">
+        <v>3</v>
+      </c>
+      <c r="I90">
+        <f t="shared" ref="I90:I127" si="30">D90*H90</f>
+        <v>3</v>
+      </c>
+      <c r="J90">
+        <f>J89+I90</f>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91" s="3">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="G91">
+        <f t="shared" ref="G91:G97" si="31">G90+F91</f>
+        <v>187</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="J91">
+        <f t="shared" ref="J91:J127" si="32">J90+I91</f>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92" s="3">
+        <v>3</v>
+      </c>
+      <c r="D92" s="3">
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <v>7</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="29"/>
+        <v>21</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="31"/>
+        <v>208</v>
+      </c>
+      <c r="H92">
+        <v>7</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="30"/>
+        <v>21</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="32"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>5</v>
+      </c>
+      <c r="C93" s="3">
+        <v>9</v>
+      </c>
+      <c r="D93" s="3">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="29"/>
+        <v>27</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="31"/>
+        <v>235</v>
+      </c>
+      <c r="H93">
+        <v>3</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="30"/>
+        <v>27</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="32"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>6</v>
+      </c>
+      <c r="C94" s="3">
+        <v>8</v>
+      </c>
+      <c r="D94" s="3">
+        <v>8</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="31"/>
+        <v>243</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="30"/>
+        <v>8</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="32"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>7</v>
+      </c>
+      <c r="C95" s="3">
+        <v>7</v>
+      </c>
+      <c r="D95" s="3">
+        <v>7</v>
+      </c>
+      <c r="E95">
+        <v>7</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="29"/>
+        <v>49</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="31"/>
+        <v>292</v>
+      </c>
+      <c r="H95">
+        <v>7</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="30"/>
+        <v>49</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="32"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96" s="3">
+        <v>6</v>
+      </c>
+      <c r="D96" s="3">
+        <v>6</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="29"/>
+        <v>18</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="31"/>
+        <v>310</v>
+      </c>
+      <c r="H96">
+        <v>3</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="30"/>
+        <v>18</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="32"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>9</v>
+      </c>
+      <c r="C97" s="3">
+        <v>5</v>
+      </c>
+      <c r="D97" s="3">
+        <v>5</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="31"/>
+        <v>315</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="30"/>
+        <v>5</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="32"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" s="3">
+        <v>5</v>
+      </c>
+      <c r="D98" s="3">
+        <v>5</v>
+      </c>
+      <c r="H98">
+        <v>7</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="30"/>
+        <v>35</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="32"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99" s="3">
+        <v>3</v>
+      </c>
+      <c r="D99" s="3">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>7</v>
+      </c>
+      <c r="F99">
+        <f>D99*E99</f>
+        <v>21</v>
+      </c>
+      <c r="G99">
+        <f>F99</f>
+        <v>21</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="30"/>
+        <v>9</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="32"/>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" s="3">
+        <v>3</v>
+      </c>
+      <c r="D100" s="3">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100">
+        <f t="shared" ref="F100:F104" si="33">D100*E100</f>
+        <v>9</v>
+      </c>
+      <c r="G100">
+        <f>G99+F100</f>
+        <v>30</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="32"/>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="G101">
+        <f t="shared" ref="G101:G104" si="34">G100+F101</f>
+        <v>31</v>
+      </c>
+      <c r="H101">
+        <v>7</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="30"/>
+        <v>7</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="32"/>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>7</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="34"/>
+        <v>38</v>
+      </c>
+      <c r="H102">
+        <v>3</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="32"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103" s="3">
+        <v>2</v>
+      </c>
+      <c r="D103" s="3">
+        <v>2</v>
+      </c>
+      <c r="E103">
+        <v>3</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="33"/>
+        <v>6</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="34"/>
+        <v>44</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="32"/>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>6</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2</v>
+      </c>
+      <c r="D104" s="3">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="34"/>
+        <v>46</v>
+      </c>
+      <c r="H104">
+        <v>7</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="30"/>
+        <v>14</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="32"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>15</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" s="3">
+        <v>6</v>
+      </c>
+      <c r="D105" s="3">
+        <v>6</v>
+      </c>
+      <c r="H105">
+        <v>3</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="30"/>
+        <v>18</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="32"/>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2</v>
+      </c>
+      <c r="D106" s="3">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>7</v>
+      </c>
+      <c r="F106">
+        <f>D106*E106</f>
+        <v>14</v>
+      </c>
+      <c r="G106">
+        <f>F106</f>
+        <v>14</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="32"/>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" s="3">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>3</v>
+      </c>
+      <c r="F107">
+        <f t="shared" ref="F107:F111" si="35">D107*E107</f>
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <f>G106+F107</f>
+        <v>14</v>
+      </c>
+      <c r="H107">
+        <v>7</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="32"/>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <f t="shared" ref="G108:G111" si="36">G107+F108</f>
+        <v>15</v>
+      </c>
+      <c r="H108">
+        <v>3</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="32"/>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>4</v>
+      </c>
+      <c r="C109" s="3">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>7</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="36"/>
+        <v>15</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="32"/>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>5</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2</v>
+      </c>
+      <c r="D110" s="3">
+        <v>2</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="36"/>
+        <v>21</v>
+      </c>
+      <c r="H110">
+        <v>7</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="30"/>
+        <v>14</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="32"/>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>6</v>
+      </c>
+      <c r="C111" s="3">
+        <v>0</v>
+      </c>
+      <c r="D111" s="3">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="36"/>
+        <v>21</v>
+      </c>
+      <c r="H111">
+        <v>3</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="32"/>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112" s="3">
+        <v>1</v>
+      </c>
+      <c r="D112" s="3">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" s="3">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>7</v>
+      </c>
+      <c r="F113">
+        <f>D113*E113</f>
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <f>F113</f>
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>7</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" s="3">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>3</v>
+      </c>
+      <c r="F114">
+        <f t="shared" ref="F114:F126" si="37">D114*E114</f>
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <f>G113+F114</f>
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>3</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" s="3">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <f t="shared" ref="G115:G126" si="38">G114+F115</f>
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>4</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" s="3">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>7</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>7</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>5</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" s="3">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>3</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>3</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>6</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D118" s="3">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>7</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D119" s="3">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>7</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>7</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D120" s="3">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>3</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>3</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>9</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>7</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>7</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>11</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D123" s="3">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>3</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>3</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>12</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D124" s="3">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>13</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D125" s="3">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>7</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>7</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>14</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" s="3">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>3</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>3</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>19</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" s="3">
+        <v>0</v>
+      </c>
+      <c r="D127" s="3">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="32"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128">
+        <v>6</v>
+      </c>
       <c r="C128" s="3"/>
+    </row>
+    <row r="131" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I131" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K131" s="2"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D132">
+        <v>28</v>
+      </c>
+      <c r="E132">
+        <v>7</v>
+      </c>
+      <c r="F132">
+        <f>D132*E132</f>
+        <v>196</v>
+      </c>
+      <c r="G132">
+        <f>F132</f>
+        <v>196</v>
+      </c>
+      <c r="H132">
+        <v>7</v>
+      </c>
+      <c r="I132">
+        <f>D132*H132</f>
+        <v>196</v>
+      </c>
+      <c r="J132">
+        <f>I132</f>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D133" s="3">
+        <v>29</v>
+      </c>
+      <c r="E133">
+        <v>3</v>
+      </c>
+      <c r="F133">
+        <f t="shared" ref="F133:F140" si="39">D133*E133</f>
+        <v>87</v>
+      </c>
+      <c r="G133">
+        <f>G132+F133</f>
+        <v>283</v>
+      </c>
+      <c r="H133">
+        <v>3</v>
+      </c>
+      <c r="I133">
+        <f t="shared" ref="I133:I170" si="40">D133*H133</f>
+        <v>87</v>
+      </c>
+      <c r="J133">
+        <f>J132+I133</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>3</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D134" s="3">
+        <v>10</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="39"/>
+        <v>10</v>
+      </c>
+      <c r="G134">
+        <f t="shared" ref="G134:G140" si="41">G133+F134</f>
+        <v>293</v>
+      </c>
+      <c r="H134">
+        <v>1</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="J134">
+        <f t="shared" ref="J134:J170" si="42">J133+I134</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>4</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D135" s="3">
+        <v>27</v>
+      </c>
+      <c r="E135">
+        <v>7</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="39"/>
+        <v>189</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="41"/>
+        <v>482</v>
+      </c>
+      <c r="H135">
+        <v>7</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="40"/>
+        <v>189</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="42"/>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>5</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D136" s="3">
+        <v>32</v>
+      </c>
+      <c r="E136">
+        <v>3</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="39"/>
+        <v>96</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="41"/>
+        <v>578</v>
+      </c>
+      <c r="H136">
+        <v>3</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="40"/>
+        <v>96</v>
+      </c>
+      <c r="J136">
+        <f t="shared" si="42"/>
+        <v>578</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>6</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" s="3">
+        <v>10</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="39"/>
+        <v>10</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="41"/>
+        <v>588</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="J137">
+        <f t="shared" si="42"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>7</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" s="3">
+        <v>27</v>
+      </c>
+      <c r="E138">
+        <v>7</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="39"/>
+        <v>189</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="41"/>
+        <v>777</v>
+      </c>
+      <c r="H138">
+        <v>7</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="40"/>
+        <v>189</v>
+      </c>
+      <c r="J138">
+        <f t="shared" si="42"/>
+        <v>777</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>8</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D139" s="3">
+        <v>28</v>
+      </c>
+      <c r="E139">
+        <v>3</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="39"/>
+        <v>84</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="41"/>
+        <v>861</v>
+      </c>
+      <c r="H139">
+        <v>3</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="40"/>
+        <v>84</v>
+      </c>
+      <c r="J139">
+        <f t="shared" si="42"/>
+        <v>861</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>9</v>
+      </c>
+      <c r="C140" s="3">
+        <v>4</v>
+      </c>
+      <c r="D140" s="3">
+        <v>4</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="39"/>
+        <v>4</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="41"/>
+        <v>865</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+      <c r="I140">
+        <f t="shared" si="40"/>
+        <v>4</v>
+      </c>
+      <c r="J140">
+        <f t="shared" si="42"/>
+        <v>865</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>11</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" s="3">
+        <v>5</v>
+      </c>
+      <c r="D141" s="3">
+        <v>5</v>
+      </c>
+      <c r="H141">
+        <v>7</v>
+      </c>
+      <c r="I141">
+        <f t="shared" si="40"/>
+        <v>35</v>
+      </c>
+      <c r="J141">
+        <f t="shared" si="42"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" s="3">
+        <v>7</v>
+      </c>
+      <c r="D142" s="3">
+        <v>7</v>
+      </c>
+      <c r="E142">
+        <v>7</v>
+      </c>
+      <c r="F142">
+        <f>D142*E142</f>
+        <v>49</v>
+      </c>
+      <c r="G142">
+        <f>F142</f>
+        <v>49</v>
+      </c>
+      <c r="H142">
+        <v>3</v>
+      </c>
+      <c r="I142">
+        <f t="shared" si="40"/>
+        <v>21</v>
+      </c>
+      <c r="J142">
+        <f t="shared" si="42"/>
+        <v>921</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>2</v>
+      </c>
+      <c r="C143" s="3">
+        <v>7</v>
+      </c>
+      <c r="D143" s="3">
+        <v>7</v>
+      </c>
+      <c r="E143">
+        <v>3</v>
+      </c>
+      <c r="F143">
+        <f t="shared" ref="F143:F147" si="43">D143*E143</f>
+        <v>21</v>
+      </c>
+      <c r="G143">
+        <f>G142+F143</f>
+        <v>70</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <f t="shared" si="40"/>
+        <v>7</v>
+      </c>
+      <c r="J143">
+        <f t="shared" si="42"/>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>3</v>
+      </c>
+      <c r="C144" s="3">
+        <v>0</v>
+      </c>
+      <c r="D144" s="3">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <f t="shared" ref="G144:G147" si="44">G143+F144</f>
+        <v>70</v>
+      </c>
+      <c r="H144">
+        <v>7</v>
+      </c>
+      <c r="I144">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <f t="shared" si="42"/>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>4</v>
+      </c>
+      <c r="C145" s="3">
+        <v>5</v>
+      </c>
+      <c r="D145" s="3">
+        <v>5</v>
+      </c>
+      <c r="E145">
+        <v>7</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="43"/>
+        <v>35</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="44"/>
+        <v>105</v>
+      </c>
+      <c r="H145">
+        <v>3</v>
+      </c>
+      <c r="I145">
+        <f t="shared" si="40"/>
+        <v>15</v>
+      </c>
+      <c r="J145">
+        <f t="shared" si="42"/>
+        <v>943</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>5</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2</v>
+      </c>
+      <c r="D146" s="3">
+        <v>2</v>
+      </c>
+      <c r="E146">
+        <v>3</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="43"/>
+        <v>6</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="44"/>
+        <v>111</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <f t="shared" si="40"/>
+        <v>2</v>
+      </c>
+      <c r="J146">
+        <f t="shared" si="42"/>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>6</v>
+      </c>
+      <c r="C147" s="3">
+        <v>5</v>
+      </c>
+      <c r="D147" s="3">
+        <v>5</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="43"/>
+        <v>5</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="44"/>
+        <v>116</v>
+      </c>
+      <c r="H147">
+        <v>7</v>
+      </c>
+      <c r="I147">
+        <f t="shared" si="40"/>
+        <v>35</v>
+      </c>
+      <c r="J147">
+        <f t="shared" si="42"/>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>15</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148" s="3">
+        <v>6</v>
+      </c>
+      <c r="D148" s="3">
+        <v>6</v>
+      </c>
+      <c r="H148">
+        <v>3</v>
+      </c>
+      <c r="I148">
+        <f t="shared" si="40"/>
+        <v>18</v>
+      </c>
+      <c r="J148">
+        <f t="shared" si="42"/>
+        <v>998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="C149" s="3">
+        <v>2</v>
+      </c>
+      <c r="D149" s="3">
+        <v>2</v>
+      </c>
+      <c r="E149">
+        <v>7</v>
+      </c>
+      <c r="F149">
+        <f>D149*E149</f>
+        <v>14</v>
+      </c>
+      <c r="G149">
+        <f>F149</f>
+        <v>14</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="I149">
+        <f t="shared" si="40"/>
+        <v>2</v>
+      </c>
+      <c r="J149">
+        <f t="shared" si="42"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150" s="3">
+        <v>4</v>
+      </c>
+      <c r="D150" s="3">
+        <v>4</v>
+      </c>
+      <c r="E150">
+        <v>3</v>
+      </c>
+      <c r="F150">
+        <f t="shared" ref="F150:F154" si="45">D150*E150</f>
+        <v>12</v>
+      </c>
+      <c r="G150">
+        <f>G149+F150</f>
+        <v>26</v>
+      </c>
+      <c r="H150">
+        <v>7</v>
+      </c>
+      <c r="I150">
+        <f t="shared" si="40"/>
+        <v>28</v>
+      </c>
+      <c r="J150">
+        <f t="shared" si="42"/>
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>3</v>
+      </c>
+      <c r="C151" s="3">
+        <v>0</v>
+      </c>
+      <c r="D151" s="3">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <f t="shared" ref="G151:G154" si="46">G150+F151</f>
+        <v>26</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+      <c r="I151">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <f t="shared" si="42"/>
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>4</v>
+      </c>
+      <c r="C152" s="3">
+        <v>5</v>
+      </c>
+      <c r="D152" s="3">
+        <v>5</v>
+      </c>
+      <c r="E152">
+        <v>7</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="45"/>
+        <v>35</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="46"/>
+        <v>61</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <f t="shared" si="40"/>
+        <v>5</v>
+      </c>
+      <c r="J152">
+        <f t="shared" si="42"/>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>5</v>
+      </c>
+      <c r="C153" s="3">
+        <v>2</v>
+      </c>
+      <c r="D153" s="3">
+        <v>2</v>
+      </c>
+      <c r="E153">
+        <v>3</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="45"/>
+        <v>6</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="46"/>
+        <v>67</v>
+      </c>
+      <c r="H153">
+        <v>7</v>
+      </c>
+      <c r="I153">
+        <f t="shared" si="40"/>
+        <v>14</v>
+      </c>
+      <c r="J153">
+        <f t="shared" si="42"/>
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>6</v>
+      </c>
+      <c r="C154" s="3">
+        <v>5</v>
+      </c>
+      <c r="D154" s="3">
+        <v>5</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="45"/>
+        <v>5</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="46"/>
+        <v>72</v>
+      </c>
+      <c r="H154">
+        <v>3</v>
+      </c>
+      <c r="I154">
+        <f t="shared" si="40"/>
+        <v>15</v>
+      </c>
+      <c r="J154">
+        <f t="shared" si="42"/>
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>16</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155" s="3">
+        <v>2</v>
+      </c>
+      <c r="D155" s="3">
+        <v>2</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+      <c r="I155">
+        <f t="shared" si="40"/>
+        <v>2</v>
+      </c>
+      <c r="J155">
+        <f t="shared" si="42"/>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D156" s="3">
+        <v>17</v>
+      </c>
+      <c r="E156">
+        <v>7</v>
+      </c>
+      <c r="F156">
+        <f>D156*E156</f>
+        <v>119</v>
+      </c>
+      <c r="G156">
+        <f>F156</f>
+        <v>119</v>
+      </c>
+      <c r="H156">
+        <v>7</v>
+      </c>
+      <c r="I156">
+        <f t="shared" si="40"/>
+        <v>119</v>
+      </c>
+      <c r="J156">
+        <f t="shared" si="42"/>
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" s="3">
+        <v>10</v>
+      </c>
+      <c r="E157">
+        <v>3</v>
+      </c>
+      <c r="F157">
+        <f t="shared" ref="F157:F169" si="47">D157*E157</f>
+        <v>30</v>
+      </c>
+      <c r="G157">
+        <f>G156+F157</f>
+        <v>149</v>
+      </c>
+      <c r="H157">
+        <v>3</v>
+      </c>
+      <c r="I157">
+        <f t="shared" si="40"/>
+        <v>30</v>
+      </c>
+      <c r="J157">
+        <f t="shared" si="42"/>
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>3</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D158" s="3">
+        <v>23</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="47"/>
+        <v>23</v>
+      </c>
+      <c r="G158">
+        <f t="shared" ref="G158:G169" si="48">G157+F158</f>
+        <v>172</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="40"/>
+        <v>23</v>
+      </c>
+      <c r="J158">
+        <f t="shared" si="42"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>4</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D159" s="3">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>7</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="48"/>
+        <v>172</v>
+      </c>
+      <c r="H159">
+        <v>7</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <f t="shared" si="42"/>
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>5</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D160" s="3">
+        <v>28</v>
+      </c>
+      <c r="E160">
+        <v>3</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="47"/>
+        <v>84</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="48"/>
+        <v>256</v>
+      </c>
+      <c r="H160">
+        <v>3</v>
+      </c>
+      <c r="I160">
+        <f t="shared" si="40"/>
+        <v>84</v>
+      </c>
+      <c r="J160">
+        <f t="shared" si="42"/>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>6</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D161" s="3">
+        <v>17</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="47"/>
+        <v>17</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="48"/>
+        <v>273</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="I161">
+        <f t="shared" si="40"/>
+        <v>17</v>
+      </c>
+      <c r="J161">
+        <f t="shared" si="42"/>
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>7</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D162" s="3">
+        <v>24</v>
+      </c>
+      <c r="E162">
+        <v>7</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="47"/>
+        <v>168</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="48"/>
+        <v>441</v>
+      </c>
+      <c r="H162">
+        <v>7</v>
+      </c>
+      <c r="I162">
+        <f t="shared" si="40"/>
+        <v>168</v>
+      </c>
+      <c r="J162">
+        <f t="shared" si="42"/>
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>8</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D163" s="3">
+        <v>29</v>
+      </c>
+      <c r="E163">
+        <v>3</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="47"/>
+        <v>87</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="48"/>
+        <v>528</v>
+      </c>
+      <c r="H163">
+        <v>3</v>
+      </c>
+      <c r="I163">
+        <f t="shared" si="40"/>
+        <v>87</v>
+      </c>
+      <c r="J163">
+        <f t="shared" si="42"/>
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>9</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" s="3">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="48"/>
+        <v>528</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J164">
+        <f t="shared" si="42"/>
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>10</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D165" s="3">
+        <v>15</v>
+      </c>
+      <c r="E165">
+        <v>7</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="47"/>
+        <v>105</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="48"/>
+        <v>633</v>
+      </c>
+      <c r="H165">
+        <v>7</v>
+      </c>
+      <c r="I165">
+        <f t="shared" si="40"/>
+        <v>105</v>
+      </c>
+      <c r="J165">
+        <f t="shared" si="42"/>
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>11</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D166" s="3">
+        <v>18</v>
+      </c>
+      <c r="E166">
+        <v>3</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="47"/>
+        <v>54</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="48"/>
+        <v>687</v>
+      </c>
+      <c r="H166">
+        <v>3</v>
+      </c>
+      <c r="I166">
+        <f t="shared" si="40"/>
+        <v>54</v>
+      </c>
+      <c r="J166">
+        <f t="shared" si="42"/>
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>12</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D167" s="3">
+        <v>27</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="47"/>
+        <v>27</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="48"/>
+        <v>714</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+      <c r="I167">
+        <f t="shared" si="40"/>
+        <v>27</v>
+      </c>
+      <c r="J167">
+        <f t="shared" si="42"/>
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>13</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D168" s="3">
+        <v>28</v>
+      </c>
+      <c r="E168">
+        <v>7</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="47"/>
+        <v>196</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="48"/>
+        <v>910</v>
+      </c>
+      <c r="H168">
+        <v>7</v>
+      </c>
+      <c r="I168">
+        <f t="shared" si="40"/>
+        <v>196</v>
+      </c>
+      <c r="J168">
+        <f t="shared" si="42"/>
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>14</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D169" s="3">
+        <v>29</v>
+      </c>
+      <c r="E169">
+        <v>3</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="47"/>
+        <v>87</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="48"/>
+        <v>997</v>
+      </c>
+      <c r="H169">
+        <v>3</v>
+      </c>
+      <c r="I169">
+        <f t="shared" si="40"/>
+        <v>87</v>
+      </c>
+      <c r="J169">
+        <f t="shared" si="42"/>
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>19</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170" s="3">
+        <v>7</v>
+      </c>
+      <c r="D170" s="3">
+        <v>7</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+      <c r="I170">
+        <f t="shared" si="40"/>
+        <v>7</v>
+      </c>
+      <c r="J170">
+        <f t="shared" si="42"/>
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>20</v>
+      </c>
+      <c r="B171">
+        <v>8</v>
+      </c>
+      <c r="C171" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Icao9302SizeTD1Algorithm Validate method and unit tests (except support for extended document numbers > 9 characters)
</commit_message>
<xml_diff>
--- a/Documentation/ICAO9303ExamplesWorkbook.xlsx
+++ b/Documentation/ICAO9303ExamplesWorkbook.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC2A28-AF27-45E9-8769-89F8D5FA0981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219E0190-68D9-4EB3-B73C-3E74D7762C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{733EF23D-49B3-4624-B260-D0D00364A32A}"/>
   </bookViews>
   <sheets>
-    <sheet name="TD3" sheetId="1" r:id="rId1"/>
+    <sheet name="TD1" sheetId="2" r:id="rId1"/>
+    <sheet name="TD3" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
   <si>
     <t>Char</t>
   </si>
@@ -144,6 +145,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -536,11 +540,1686 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B9E49F-789F-4215-8BE5-87924539EF63}">
+  <dimension ref="A2:K55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3</f>
+        <v>91</v>
+      </c>
+      <c r="G3">
+        <f>F3</f>
+        <v>91</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <f>D3*H3</f>
+        <v>91</v>
+      </c>
+      <c r="J3">
+        <f>I3</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F11" si="0">D4*E4</f>
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <f>G3+F4</f>
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I26" si="1">D4*H4</f>
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <f>J3+I4</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G11" si="2">G4+F5</f>
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J26" si="3">J4+I5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <f>D13*E13</f>
+        <v>49</v>
+      </c>
+      <c r="G13">
+        <f>F13</f>
+        <v>49</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F18" si="4">D14*E14</f>
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <f>G13+F14</f>
+        <v>61</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G18" si="5">G14+F15</f>
+        <v>61</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>122</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <f>D20*E20</f>
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <f>F20</f>
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F25" si="6">D21*E21</f>
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <f>G20+F21</f>
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G25" si="7">G21+F22</f>
+        <v>13</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>41</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <f>D31*E31</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>F31</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <f>D31*H31</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f>I31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ref="F32:F39" si="8">D32*E32</f>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f>G31+F32</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I54" si="9">D32*H32</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>J31+I32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G39" si="10">G32+F33</f>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ref="J33:J54" si="11">J32+I33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>7</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>7</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f>MOD(G39,10)</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>C40</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <f>D41*E41</f>
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f>F41</f>
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ref="F42:F46" si="12">D42*E42</f>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f>G41+F42</f>
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43:G46" si="13">G42+F43</f>
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>7</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3">
+        <f>MOD(G46,10)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <f>C47</f>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3">
+        <v>8</v>
+      </c>
+      <c r="D48" s="3">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <f>D48*E48</f>
+        <v>56</v>
+      </c>
+      <c r="G48">
+        <f>F48</f>
+        <v>56</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49:F53" si="14">D49*E49</f>
+        <v>24</v>
+      </c>
+      <c r="G49">
+        <f>G48+F49</f>
+        <v>80</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="9"/>
+        <v>56</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ref="G50:G53" si="15">G49+F50</f>
+        <v>81</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="11"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="15"/>
+        <v>95</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="11"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="15"/>
+        <v>101</v>
+      </c>
+      <c r="H52">
+        <v>7</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="11"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" s="3">
+        <v>7</v>
+      </c>
+      <c r="D53" s="3">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="15"/>
+        <v>108</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="11"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3">
+        <f>MOD(G53,10)</f>
+        <v>8</v>
+      </c>
+      <c r="D54" s="3">
+        <f>C54</f>
+        <v>8</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="11"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3">
+        <f>MOD(J54,10)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7BF346-6A22-4B48-81BB-0FB387D62345}">
   <dimension ref="A2:K171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update to handle extended document number
</commit_message>
<xml_diff>
--- a/Documentation/ICAO9303ExamplesWorkbook.xlsx
+++ b/Documentation/ICAO9303ExamplesWorkbook.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219E0190-68D9-4EB3-B73C-3E74D7762C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5244432E-5EF1-47E3-8137-6A0E830E681D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{733EF23D-49B3-4624-B260-D0D00364A32A}"/>
   </bookViews>
   <sheets>
     <sheet name="TD1" sheetId="2" r:id="rId1"/>
-    <sheet name="TD3" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="TD3" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="41">
   <si>
     <t>Char</t>
   </si>
@@ -149,6 +150,18 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>Extended Document Number Examples</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Line #</t>
+  </si>
+  <si>
+    <t>Char Pos</t>
+  </si>
 </sst>
 </file>
 
@@ -200,13 +213,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,1671 +555,3172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B9E49F-789F-4215-8BE5-87924539EF63}">
-  <dimension ref="A2:K55"/>
+  <dimension ref="A2:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>13</v>
       </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <f>D3*E3</f>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <f>F3*G3</f>
         <v>91</v>
       </c>
-      <c r="G3">
-        <f>F3</f>
+      <c r="I3">
+        <f>H3</f>
         <v>91</v>
       </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <f>D3*H3</f>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <f>F3*J3</f>
         <v>91</v>
       </c>
-      <c r="J3">
-        <f>I3</f>
+      <c r="L3">
+        <f>K3</f>
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F11" si="0">D4*E4</f>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="0">F4*G4</f>
         <v>6</v>
       </c>
-      <c r="G4">
-        <f>G3+F4</f>
+      <c r="I4">
+        <f>I3+H4</f>
         <v>97</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I26" si="1">D4*H4</f>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K26" si="1">F4*J4</f>
         <v>6</v>
       </c>
-      <c r="J4">
-        <f>J3+I4</f>
+      <c r="L4">
+        <f>L3+K4</f>
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G11" si="2">G4+F5</f>
+      <c r="I5">
+        <f t="shared" ref="I5:I11" si="2">I4+H5</f>
         <v>100</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J26" si="3">J4+I5</f>
+      <c r="L5">
+        <f t="shared" ref="L5:L26" si="3">L4+K5</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <f t="shared" si="3"/>
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>5</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <f t="shared" si="3"/>
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>8</v>
       </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>9</v>
       </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <f t="shared" si="2"/>
         <v>207</v>
       </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <f t="shared" si="2"/>
         <v>207</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
       <c r="D12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <f>D13*E13</f>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f>F13*G13</f>
         <v>49</v>
       </c>
-      <c r="G13">
-        <f>F13</f>
+      <c r="I13">
+        <f>H13</f>
         <v>49</v>
       </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13">
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <f t="shared" si="3"/>
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
         <v>4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="F14" s="3">
         <v>4</v>
       </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="F14:F18" si="4">D14*E14</f>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H18" si="4">F14*G14</f>
         <v>12</v>
       </c>
-      <c r="G14">
-        <f>G13+F14</f>
+      <c r="I14">
+        <f>I13+H14</f>
         <v>61</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <f t="shared" si="3"/>
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G15">
-        <f t="shared" ref="G15:G18" si="5">G14+F15</f>
+      <c r="I15">
+        <f t="shared" ref="I15:I18" si="5">I14+H15</f>
         <v>61</v>
       </c>
-      <c r="H15">
-        <v>7</v>
-      </c>
-      <c r="I15">
+      <c r="J15">
+        <v>7</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <f t="shared" si="3"/>
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16">
         <v>4</v>
       </c>
-      <c r="C16" s="3">
+      <c r="E16" s="3">
         <v>8</v>
       </c>
-      <c r="D16" s="3">
+      <c r="F16" s="3">
         <v>8</v>
       </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="F16">
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <f t="shared" si="5"/>
         <v>117</v>
       </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16">
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <f t="shared" si="3"/>
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D17">
         <v>5</v>
       </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <f t="shared" si="3"/>
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D18">
         <v>6</v>
       </c>
-      <c r="C18" s="3">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <f t="shared" si="5"/>
         <v>122</v>
       </c>
-      <c r="H18">
-        <v>7</v>
-      </c>
-      <c r="I18">
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <f t="shared" si="3"/>
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <f t="shared" si="3"/>
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <f>D20*E20</f>
-        <v>7</v>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
       </c>
       <c r="G20">
-        <f>F20</f>
         <v>7</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <f>F20*G20</f>
+        <v>7</v>
       </c>
       <c r="I20">
+        <f>H20</f>
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <f t="shared" si="3"/>
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <f t="shared" ref="F21:F25" si="6">D21*E21</f>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H25" si="6">F21*G21</f>
         <v>6</v>
       </c>
-      <c r="G21">
-        <f>G20+F21</f>
+      <c r="I21">
+        <f>I20+H21</f>
         <v>13</v>
       </c>
-      <c r="H21">
-        <v>7</v>
-      </c>
-      <c r="I21">
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <f t="shared" si="3"/>
         <v>341</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:G25" si="7">G21+F22</f>
+      <c r="I22">
+        <f t="shared" ref="I22:I25" si="7">I21+H22</f>
         <v>13</v>
       </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22">
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <f t="shared" si="3"/>
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D23">
         <v>4</v>
       </c>
-      <c r="C23" s="3">
+      <c r="E23" s="3">
         <v>4</v>
       </c>
-      <c r="D23" s="3">
+      <c r="F23" s="3">
         <v>4</v>
       </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="F23">
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <f t="shared" si="7"/>
         <v>41</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <f t="shared" si="3"/>
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D24">
         <v>5</v>
       </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="F24">
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <f t="shared" si="7"/>
         <v>44</v>
       </c>
-      <c r="H24">
-        <v>7</v>
-      </c>
-      <c r="I24">
+      <c r="J24">
+        <v>7</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <f t="shared" si="3"/>
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D25">
         <v>6</v>
       </c>
-      <c r="C25" s="3">
+      <c r="E25" s="3">
         <v>5</v>
       </c>
-      <c r="D25" s="3">
+      <c r="F25" s="3">
         <v>5</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <f t="shared" si="7"/>
         <v>49</v>
       </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25">
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <f t="shared" si="3"/>
         <v>367</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
         <v>9</v>
       </c>
-      <c r="D26" s="3">
+      <c r="F26" s="3">
         <v>9</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <f t="shared" si="3"/>
         <v>376</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="I30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <f>D31*E31</f>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
         <v>0</v>
       </c>
       <c r="G31">
-        <f>F31</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H31">
-        <v>7</v>
+        <f>F31*G31</f>
+        <v>0</v>
       </c>
       <c r="I31">
-        <f>D31*H31</f>
+        <f>H31</f>
         <v>0</v>
       </c>
       <c r="J31">
-        <f>I31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <f t="shared" ref="F32:F39" si="8">D32*E32</f>
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <f>F31*J31</f>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f>K31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
         <v>0</v>
       </c>
       <c r="G32">
-        <f>G31+F32</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <f t="shared" ref="H32:H39" si="8">F32*G32</f>
+        <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I32:I54" si="9">D32*H32</f>
+        <f>I31+H32</f>
         <v>0</v>
       </c>
       <c r="J32">
-        <f>J31+I32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:K54" si="9">F32*J32</f>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>L31+K32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G33">
-        <f t="shared" ref="G33:G39" si="10">G32+F33</f>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
       <c r="I33">
+        <f t="shared" ref="I33:I39" si="10">I32+H33</f>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J33">
-        <f t="shared" ref="J33:J54" si="11">J32+I33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="L33">
+        <f t="shared" ref="L33:L54" si="11">L32+K33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D34">
         <v>4</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>7</v>
-      </c>
-      <c r="F34">
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>7</v>
-      </c>
-      <c r="I34">
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D35">
         <v>5</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35">
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H35">
-        <v>3</v>
-      </c>
-      <c r="I35">
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D36">
         <v>6</v>
       </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>7</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
-      </c>
-      <c r="F37">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H37">
-        <v>7</v>
-      </c>
-      <c r="I37">
+      <c r="J37">
+        <v>7</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D38">
         <v>8</v>
       </c>
-      <c r="C38" s="3">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38">
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H38">
-        <v>3</v>
-      </c>
-      <c r="I38">
+      <c r="J38">
+        <v>3</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D39">
         <v>9</v>
       </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <f>MOD(G39,10)</f>
-        <v>0</v>
-      </c>
       <c r="D40">
-        <f>C40</f>
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>7</v>
-      </c>
-      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <f>MOD(I39,10)</f>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f>E40</f>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J40">
+      <c r="L40">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3">
-        <v>0</v>
-      </c>
-      <c r="D41" s="3">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <f>D41*E41</f>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
         <v>0</v>
       </c>
       <c r="G41">
-        <f>F41</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <f>F41*G41</f>
+        <v>0</v>
       </c>
       <c r="I41">
+        <f>H41</f>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" s="3">
-        <v>0</v>
-      </c>
-      <c r="D42" s="3">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>3</v>
-      </c>
-      <c r="F42">
-        <f t="shared" ref="F42:F46" si="12">D42*E42</f>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
         <v>0</v>
       </c>
       <c r="G42">
-        <f>G41+F42</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <f t="shared" ref="H42:H46" si="12">F42*G42</f>
+        <v>0</v>
       </c>
       <c r="I42">
+        <f>I41+H42</f>
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43" s="3">
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G43">
-        <f t="shared" ref="G43:G46" si="13">G42+F43</f>
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>7</v>
-      </c>
       <c r="I43">
+        <f t="shared" ref="I43:I46" si="13">I42+H43</f>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>7</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D44">
         <v>4</v>
       </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>7</v>
-      </c>
-      <c r="F44">
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G44">
+      <c r="I44">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H44">
-        <v>3</v>
-      </c>
-      <c r="I44">
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D45">
         <v>5</v>
       </c>
-      <c r="C45" s="3">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>3</v>
-      </c>
-      <c r="F45">
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G45">
+      <c r="I45">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45">
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D46">
         <v>6</v>
       </c>
-      <c r="C46" s="3">
-        <v>0</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G46">
+      <c r="I46">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H46">
-        <v>7</v>
-      </c>
-      <c r="I46">
+      <c r="J46">
+        <v>7</v>
+      </c>
+      <c r="K46">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>15</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3">
-        <f>MOD(G46,10)</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="3">
-        <f>C47</f>
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>3</v>
-      </c>
-      <c r="I47">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <f>MOD(I46,10)</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <f>E47</f>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
         <v>8</v>
       </c>
-      <c r="D48" s="3">
+      <c r="F48" s="3">
         <v>8</v>
       </c>
-      <c r="E48">
-        <v>7</v>
-      </c>
-      <c r="F48">
-        <f>D48*E48</f>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48">
+        <f>F48*G48</f>
         <v>56</v>
       </c>
-      <c r="G48">
-        <f>F48</f>
+      <c r="I48">
+        <f>H48</f>
         <v>56</v>
       </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48">
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>2</v>
-      </c>
-      <c r="C49" s="3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
         <v>8</v>
       </c>
-      <c r="D49" s="3">
+      <c r="F49" s="3">
         <v>8</v>
       </c>
-      <c r="E49">
-        <v>3</v>
-      </c>
-      <c r="F49">
-        <f t="shared" ref="F49:F53" si="14">D49*E49</f>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49:H53" si="14">F49*G49</f>
         <v>24</v>
       </c>
-      <c r="G49">
-        <f>G48+F49</f>
+      <c r="I49">
+        <f>I48+H49</f>
         <v>80</v>
       </c>
-      <c r="H49">
-        <v>7</v>
-      </c>
-      <c r="I49">
+      <c r="J49">
+        <v>7</v>
+      </c>
+      <c r="K49">
         <f t="shared" si="9"/>
         <v>56</v>
       </c>
-      <c r="J49">
+      <c r="L49">
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="G50">
-        <f t="shared" ref="G50:G53" si="15">G49+F50</f>
+      <c r="I50">
+        <f t="shared" ref="I50:I53" si="15">I49+H50</f>
         <v>81</v>
       </c>
-      <c r="H50">
-        <v>3</v>
-      </c>
-      <c r="I50">
+      <c r="J50">
+        <v>3</v>
+      </c>
+      <c r="K50">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="J50">
+      <c r="L50">
         <f t="shared" si="11"/>
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B51">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D51">
         <v>4</v>
       </c>
-      <c r="C51" s="3">
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <v>2</v>
-      </c>
-      <c r="E51">
-        <v>7</v>
-      </c>
-      <c r="F51">
+      <c r="E51" s="3">
+        <v>2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>7</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="G51">
+      <c r="I51">
         <f t="shared" si="15"/>
         <v>95</v>
       </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="I51">
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="J51">
+      <c r="L51">
         <f t="shared" si="11"/>
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D52">
         <v>5</v>
       </c>
-      <c r="C52" s="3">
-        <v>2</v>
-      </c>
-      <c r="D52" s="3">
-        <v>2</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
-      <c r="F52">
+      <c r="E52" s="3">
+        <v>2</v>
+      </c>
+      <c r="F52" s="3">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="14"/>
         <v>6</v>
       </c>
-      <c r="G52">
+      <c r="I52">
         <f t="shared" si="15"/>
         <v>101</v>
       </c>
-      <c r="H52">
-        <v>7</v>
-      </c>
-      <c r="I52">
+      <c r="J52">
+        <v>7</v>
+      </c>
+      <c r="K52">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="J52">
+      <c r="L52">
         <f t="shared" si="11"/>
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D53">
         <v>6</v>
       </c>
-      <c r="C53" s="3">
-        <v>7</v>
-      </c>
-      <c r="D53" s="3">
-        <v>7</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53">
+      <c r="E53" s="3">
+        <v>7</v>
+      </c>
+      <c r="F53" s="3">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
         <f t="shared" si="14"/>
         <v>7</v>
       </c>
-      <c r="G53">
+      <c r="I53">
         <f t="shared" si="15"/>
         <v>108</v>
       </c>
-      <c r="H53">
-        <v>3</v>
-      </c>
-      <c r="I53">
+      <c r="J53">
+        <v>3</v>
+      </c>
+      <c r="K53">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <f t="shared" si="11"/>
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" s="3">
-        <f>MOD(G53,10)</f>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <f>MOD(I53,10)</f>
         <v>8</v>
       </c>
-      <c r="D54" s="3">
-        <f>C54</f>
+      <c r="F54" s="3">
+        <f>E54</f>
         <v>8</v>
       </c>
-      <c r="H54">
-        <v>1</v>
-      </c>
-      <c r="I54">
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="J54">
+      <c r="L54">
         <f t="shared" si="11"/>
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" s="3">
-        <f>MOD(J54,10)</f>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <f>MOD(L54,10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61">
+        <v>13</v>
+      </c>
+      <c r="G61">
+        <v>7</v>
+      </c>
+      <c r="H61">
+        <f>F61*G61</f>
+        <v>91</v>
+      </c>
+      <c r="I61">
+        <f>H61</f>
+        <v>91</v>
+      </c>
+      <c r="J61">
+        <v>7</v>
+      </c>
+      <c r="K61">
+        <f>F61*J61</f>
+        <v>91</v>
+      </c>
+      <c r="L61">
+        <f>K61</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <f t="shared" ref="H62:H68" si="16">F62*G62</f>
+        <v>6</v>
+      </c>
+      <c r="I62">
+        <f>I61+H62</f>
+        <v>97</v>
+      </c>
+      <c r="J62">
+        <v>3</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62:K97" si="17">F62*J62</f>
+        <v>6</v>
+      </c>
+      <c r="L62">
+        <f>L61+K62</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I63">
+        <f t="shared" ref="I63:I68" si="18">I62+H63</f>
+        <v>100</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="L63">
+        <f t="shared" ref="L63:L97" si="19">L62+K63</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>7</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="18"/>
+        <v>107</v>
+      </c>
+      <c r="J64">
+        <v>7</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="19"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>4</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="18"/>
+        <v>119</v>
+      </c>
+      <c r="J65">
+        <v>3</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="19"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66">
+        <v>5</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="18"/>
+        <v>124</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="19"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
+        <v>8</v>
+      </c>
+      <c r="G67">
+        <v>7</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="16"/>
+        <v>56</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="18"/>
+        <v>180</v>
+      </c>
+      <c r="J67">
+        <v>7</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="17"/>
+        <v>56</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="19"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>8</v>
+      </c>
+      <c r="E68">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>9</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="18"/>
+        <v>207</v>
+      </c>
+      <c r="J68">
+        <v>3</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="17"/>
+        <v>27</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="19"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>9</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <f t="shared" ref="H69:H82" si="20">F69*G69</f>
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <f t="shared" ref="I69:I82" si="21">I68+H69</f>
+        <v>207</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <f t="shared" ref="K69:K82" si="22">F69*J69</f>
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <f t="shared" ref="L69:L82" si="23">L68+K69</f>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>16</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" s="3">
+        <v>10</v>
+      </c>
+      <c r="G70">
+        <v>7</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="20"/>
+        <v>70</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="21"/>
+        <v>277</v>
+      </c>
+      <c r="J70">
+        <v>7</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="22"/>
+        <v>70</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="23"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>17</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="3">
+        <v>11</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="20"/>
+        <v>33</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="21"/>
+        <v>310</v>
+      </c>
+      <c r="J71">
+        <v>3</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="22"/>
+        <v>33</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="23"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>18</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="21"/>
+        <v>311</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="23"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>19</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73" s="3">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>7</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="21"/>
+        <v>318</v>
+      </c>
+      <c r="J73">
+        <v>7</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="22"/>
+        <v>7</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="23"/>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>20</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74" s="3">
+        <v>2</v>
+      </c>
+      <c r="F74" s="3">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="20"/>
+        <v>6</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="21"/>
+        <v>324</v>
+      </c>
+      <c r="J74">
+        <v>3</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="22"/>
+        <v>6</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="23"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>21</v>
+      </c>
+      <c r="D75">
+        <v>6</v>
+      </c>
+      <c r="E75" s="3">
+        <v>2</v>
+      </c>
+      <c r="F75" s="3">
+        <v>2</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="21"/>
+        <v>326</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="23"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>22</v>
+      </c>
+      <c r="D76">
+        <v>7</v>
+      </c>
+      <c r="E76" s="3">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3">
+        <v>3</v>
+      </c>
+      <c r="G76">
+        <v>7</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="20"/>
+        <v>21</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="21"/>
+        <v>347</v>
+      </c>
+      <c r="J76">
+        <v>7</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="22"/>
+        <v>21</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="23"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>23</v>
+      </c>
+      <c r="D77">
+        <v>8</v>
+      </c>
+      <c r="E77" s="3">
+        <v>8</v>
+      </c>
+      <c r="F77" s="3">
+        <v>8</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="20"/>
+        <v>24</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="21"/>
+        <v>371</v>
+      </c>
+      <c r="J77">
+        <v>3</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="22"/>
+        <v>24</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="23"/>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>24</v>
+      </c>
+      <c r="D78">
+        <v>9</v>
+      </c>
+      <c r="E78" s="3">
+        <v>5</v>
+      </c>
+      <c r="F78" s="3">
+        <v>5</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="21"/>
+        <v>376</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="23"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>25</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+      <c r="E79" s="3">
+        <v>6</v>
+      </c>
+      <c r="F79" s="3">
+        <v>6</v>
+      </c>
+      <c r="G79">
+        <v>7</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="20"/>
+        <v>42</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="21"/>
+        <v>418</v>
+      </c>
+      <c r="J79">
+        <v>7</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="23"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>26</v>
+      </c>
+      <c r="D80">
+        <v>11</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="21"/>
+        <v>418</v>
+      </c>
+      <c r="J80">
+        <v>3</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="23"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>27</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81" s="3">
+        <v>0</v>
+      </c>
+      <c r="F81" s="3">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="21"/>
+        <v>418</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="23"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>28</v>
+      </c>
+      <c r="D82">
+        <v>13</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>7</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="21"/>
+        <v>418</v>
+      </c>
+      <c r="J82">
+        <v>7</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="23"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>29</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <f>MOD(L82,10)</f>
+        <v>8</v>
+      </c>
+      <c r="F83">
+        <f>E83</f>
+        <v>8</v>
+      </c>
+      <c r="J83">
+        <v>3</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="L83">
+        <f>L82+K83</f>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" s="3">
+        <v>7</v>
+      </c>
+      <c r="F84" s="3">
+        <v>7</v>
+      </c>
+      <c r="G84">
+        <v>7</v>
+      </c>
+      <c r="H84">
+        <f>F84*G84</f>
+        <v>49</v>
+      </c>
+      <c r="I84">
+        <f>H84</f>
+        <v>49</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="19"/>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85" s="3">
+        <v>4</v>
+      </c>
+      <c r="F85" s="3">
+        <v>4</v>
+      </c>
+      <c r="G85">
+        <v>3</v>
+      </c>
+      <c r="H85">
+        <f t="shared" ref="H85:H89" si="24">F85*G85</f>
+        <v>12</v>
+      </c>
+      <c r="I85">
+        <f>I84+H85</f>
+        <v>61</v>
+      </c>
+      <c r="J85">
+        <v>7</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="17"/>
+        <v>28</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="19"/>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <f t="shared" ref="I86:I89" si="25">I85+H86</f>
+        <v>61</v>
+      </c>
+      <c r="J86">
+        <v>3</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="19"/>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87" s="3">
+        <v>8</v>
+      </c>
+      <c r="F87" s="3">
+        <v>8</v>
+      </c>
+      <c r="G87">
+        <v>7</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="24"/>
+        <v>56</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="25"/>
+        <v>117</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="19"/>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="25"/>
+        <v>120</v>
+      </c>
+      <c r="J88">
+        <v>7</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="19"/>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+      <c r="D89">
+        <v>6</v>
+      </c>
+      <c r="E89" s="3">
+        <v>2</v>
+      </c>
+      <c r="F89" s="3">
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="25"/>
+        <v>122</v>
+      </c>
+      <c r="J89">
+        <v>3</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="19"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>7</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90" s="3">
+        <v>2</v>
+      </c>
+      <c r="F90" s="3">
+        <v>2</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="19"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>9</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" s="3">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>7</v>
+      </c>
+      <c r="H91">
+        <f>F91*G91</f>
+        <v>7</v>
+      </c>
+      <c r="I91">
+        <f>H91</f>
+        <v>7</v>
+      </c>
+      <c r="J91">
+        <v>7</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="19"/>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92" s="3">
+        <v>2</v>
+      </c>
+      <c r="F92" s="3">
+        <v>2</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="H92">
+        <f t="shared" ref="H92:H96" si="26">F92*G92</f>
+        <v>6</v>
+      </c>
+      <c r="I92">
+        <f>I91+H92</f>
+        <v>13</v>
+      </c>
+      <c r="J92">
+        <v>3</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="19"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>11</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93" s="3">
+        <v>0</v>
+      </c>
+      <c r="F93" s="3">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <f t="shared" ref="I93:I96" si="27">I92+H93</f>
+        <v>13</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="19"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>12</v>
+      </c>
+      <c r="D94">
+        <v>4</v>
+      </c>
+      <c r="E94" s="3">
+        <v>4</v>
+      </c>
+      <c r="F94" s="3">
+        <v>4</v>
+      </c>
+      <c r="G94">
+        <v>7</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="26"/>
+        <v>28</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="27"/>
+        <v>41</v>
+      </c>
+      <c r="J94">
+        <v>7</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="17"/>
+        <v>28</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="19"/>
+        <v>541</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>13</v>
+      </c>
+      <c r="D95">
+        <v>5</v>
+      </c>
+      <c r="E95" s="3">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3">
+        <v>1</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="27"/>
+        <v>44</v>
+      </c>
+      <c r="J95">
+        <v>3</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="19"/>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>14</v>
+      </c>
+      <c r="D96">
+        <v>6</v>
+      </c>
+      <c r="E96" s="3">
+        <v>5</v>
+      </c>
+      <c r="F96" s="3">
+        <v>5</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="27"/>
+        <v>49</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="19"/>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>15</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97" s="3">
+        <f>MOD(I96,10)</f>
+        <v>9</v>
+      </c>
+      <c r="F97" s="3">
+        <f>E97</f>
+        <v>9</v>
+      </c>
+      <c r="J97">
+        <v>7</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="17"/>
+        <v>63</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="19"/>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>30</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3">
+        <f>MOD(L97,10)</f>
         <v>2</v>
       </c>
     </row>
@@ -2215,6 +3730,300 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06C2AA3-CA40-44BF-AB74-0E83CAFC1E3D}">
+  <dimension ref="A1:AD4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="30" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4">
+        <v>10</v>
+      </c>
+      <c r="K3" s="4">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4">
+        <v>13</v>
+      </c>
+      <c r="N3" s="4">
+        <v>14</v>
+      </c>
+      <c r="O3" s="4">
+        <v>15</v>
+      </c>
+      <c r="P3" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>17</v>
+      </c>
+      <c r="R3" s="4">
+        <v>18</v>
+      </c>
+      <c r="S3" s="4">
+        <v>19</v>
+      </c>
+      <c r="T3" s="4">
+        <v>20</v>
+      </c>
+      <c r="U3" s="4">
+        <v>21</v>
+      </c>
+      <c r="V3" s="4">
+        <v>22</v>
+      </c>
+      <c r="W3" s="4">
+        <v>23</v>
+      </c>
+      <c r="X3" s="4">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>25</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>27</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>29</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>9</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>7</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7BF346-6A22-4B48-81BB-0FB387D62345}">
   <dimension ref="A2:K171"/>
   <sheetViews>

</xml_diff>

<commit_message>
Validate method and associated unit tests
</commit_message>
<xml_diff>
--- a/Documentation/ICAO9303ExamplesWorkbook.xlsx
+++ b/Documentation/ICAO9303ExamplesWorkbook.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BFC6B9-B215-46B4-908F-15D60D05A36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3600CBC0-A879-4511-97CC-8AC00B7546E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{733EF23D-49B3-4624-B260-D0D00364A32A}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{733EF23D-49B3-4624-B260-D0D00364A32A}"/>
   </bookViews>
   <sheets>
     <sheet name="TD1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="TD3" sheetId="1" r:id="rId3"/>
+    <sheet name="TD2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="TD3" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="41">
   <si>
     <t>Char</t>
   </si>
@@ -557,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B9E49F-789F-4215-8BE5-87924539EF63}">
   <dimension ref="A2:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4560,6 +4561,2040 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2E5702-DCDB-4EE0-92B7-B6DAF77C1157}">
+  <dimension ref="A2:M62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <f>F3*G3</f>
+        <v>91</v>
+      </c>
+      <c r="I3">
+        <f>H3</f>
+        <v>91</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <f>F3*J3</f>
+        <v>91</v>
+      </c>
+      <c r="L3">
+        <f>K3</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="0">F4*G4</f>
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <f>I3+H4</f>
+        <v>97</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K26" si="1">F4*J4</f>
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <f>L3+K4</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I11" si="2">I4+H5</f>
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L26" si="3">L4+K5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f>F13*G13</f>
+        <v>49</v>
+      </c>
+      <c r="I13">
+        <f>H13</f>
+        <v>49</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H18" si="4">F14*G14</f>
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <f>I13+H14</f>
+        <v>61</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I18" si="5">I14+H15</f>
+        <v>61</v>
+      </c>
+      <c r="J15">
+        <v>7</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>117</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>122</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <f>F20*G20</f>
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <f>H20</f>
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H25" si="6">F21*G21</f>
+        <v>6</v>
+      </c>
+      <c r="I21">
+        <f>I20+H21</f>
+        <v>13</v>
+      </c>
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I25" si="7">I21+H22</f>
+        <v>13</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>41</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>44</v>
+      </c>
+      <c r="J24">
+        <v>7</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33">
+        <v>13</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <f>F33*G33</f>
+        <v>91</v>
+      </c>
+      <c r="I33">
+        <f>H33</f>
+        <v>91</v>
+      </c>
+      <c r="J33">
+        <v>7</v>
+      </c>
+      <c r="K33">
+        <f>F33*J33</f>
+        <v>91</v>
+      </c>
+      <c r="L33">
+        <f>K33</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:H46" si="8">F34*G34</f>
+        <v>6</v>
+      </c>
+      <c r="I34">
+        <f>I33+H34</f>
+        <v>97</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ref="K34:K61" si="9">F34*J34</f>
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <f>L33+K34</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:I46" si="10">I34+H35</f>
+        <v>100</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ref="L35:L61" si="11">L34+K35</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="10"/>
+        <v>107</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="11"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="10"/>
+        <v>119</v>
+      </c>
+      <c r="J37">
+        <v>3</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="11"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="10"/>
+        <v>124</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="11"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="10"/>
+        <v>180</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="9"/>
+        <v>56</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="11"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>9</v>
+      </c>
+      <c r="F40">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="8"/>
+        <v>27</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="10"/>
+        <v>207</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="11"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="10"/>
+        <v>207</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="11"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="3">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="10"/>
+        <v>277</v>
+      </c>
+      <c r="J42">
+        <v>7</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="9"/>
+        <v>70</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="11"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>17</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="3">
+        <v>11</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="10"/>
+        <v>310</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="9"/>
+        <v>33</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="11"/>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3">
+        <v>3</v>
+      </c>
+      <c r="F44" s="3">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="10"/>
+        <v>313</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="11"/>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45" s="3">
+        <v>8</v>
+      </c>
+      <c r="F45" s="3">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="10"/>
+        <v>369</v>
+      </c>
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="9"/>
+        <v>56</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="11"/>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="10"/>
+        <v>375</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="11"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>29</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f>MOD(I46,10)</f>
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <f>E47</f>
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="11"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>7</v>
+      </c>
+      <c r="F48" s="3">
+        <v>7</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48">
+        <f>F48*G48</f>
+        <v>49</v>
+      </c>
+      <c r="I48">
+        <f>H48</f>
+        <v>49</v>
+      </c>
+      <c r="J48">
+        <v>7</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="11"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>4</v>
+      </c>
+      <c r="F49" s="3">
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49:H53" si="12">F49*G49</f>
+        <v>12</v>
+      </c>
+      <c r="I49">
+        <f>I48+H49</f>
+        <v>61</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="11"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50:I53" si="13">I49+H50</f>
+        <v>61</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="11"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51" s="3">
+        <v>8</v>
+      </c>
+      <c r="F51" s="3">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>7</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="13"/>
+        <v>117</v>
+      </c>
+      <c r="J51">
+        <v>7</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="9"/>
+        <v>56</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="11"/>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="13"/>
+        <v>120</v>
+      </c>
+      <c r="J52">
+        <v>3</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="11"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2</v>
+      </c>
+      <c r="F53" s="3">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="13"/>
+        <v>122</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="11"/>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <f>MOD(I53,10)</f>
+        <v>2</v>
+      </c>
+      <c r="F54" s="3">
+        <f>E54</f>
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>7</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="11"/>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>9</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>7</v>
+      </c>
+      <c r="H55">
+        <f>F55*G55</f>
+        <v>7</v>
+      </c>
+      <c r="I55">
+        <f>H55</f>
+        <v>7</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="11"/>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" s="3">
+        <v>2</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:H60" si="14">F56*G56</f>
+        <v>6</v>
+      </c>
+      <c r="I56">
+        <f>I55+H56</f>
+        <v>13</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="11"/>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" ref="I57:I60" si="15">I56+H57</f>
+        <v>13</v>
+      </c>
+      <c r="J57">
+        <v>7</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="11"/>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58" s="3">
+        <v>4</v>
+      </c>
+      <c r="F58" s="3">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="14"/>
+        <v>28</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="J58">
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="11"/>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>13</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="15"/>
+        <v>44</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="11"/>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>14</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
+      <c r="E60" s="3">
+        <v>5</v>
+      </c>
+      <c r="F60" s="3">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="J60">
+        <v>7</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="9"/>
+        <v>35</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="11"/>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3">
+        <f>MOD(I60,10)</f>
+        <v>9</v>
+      </c>
+      <c r="F61" s="3">
+        <f>E61</f>
+        <v>9</v>
+      </c>
+      <c r="J61">
+        <v>3</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="11"/>
+        <v>596</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>30</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3">
+        <f>MOD(L61,10)</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06C2AA3-CA40-44BF-AB74-0E83CAFC1E3D}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
@@ -4853,7 +6888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7BF346-6A22-4B48-81BB-0FB387D62345}">
   <dimension ref="A2:K171"/>
   <sheetViews>

</xml_diff>